<commit_message>
changed training program income projection + minor adjustments
</commit_message>
<xml_diff>
--- a/estimates/shortTraining.xlsx
+++ b/estimates/shortTraining.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="G8" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>estimate</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>earnings_effect_8years_short_training</t>
+  </si>
+  <si>
+    <t>Link to appendix: https://michael-lechner.eu/ml_pdf/journals/2011_LMW-fuu_W_App_R3_081105_neu.pdf</t>
   </si>
 </sst>
 </file>
@@ -890,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -973,6 +976,9 @@
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>